<commit_message>
fixing bug on online storage calculation
</commit_message>
<xml_diff>
--- a/calc/static/piql_prices.xlsx
+++ b/calc/static/piql_prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlfredoTrujillo\PycharmProjects\calculator\calc\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6572A9-670A-40BA-9FE4-A48AB324B364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F3E634-7179-4018-B28C-32647667EEEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37410" yWindow="2970" windowWidth="14400" windowHeight="10320" tabRatio="781" xr2:uid="{D64C4359-5929-4BBC-9F5D-572B5F120BAE}"/>
+    <workbookView xWindow="28935" yWindow="1605" windowWidth="14400" windowHeight="10320" tabRatio="781" xr2:uid="{D64C4359-5929-4BBC-9F5D-572B5F120BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="prices" sheetId="13" r:id="rId1"/>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD7F3CE-3398-4BFC-A88A-63EE7D330900}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.5"/>
@@ -915,8 +915,7 @@
         <v>75</v>
       </c>
       <c r="B11" s="27">
-        <f>0.048*12</f>
-        <v>0.57600000000000007</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="C11" s="27">
         <f>0.04*12</f>
@@ -1039,6 +1038,10 @@
       <c r="C20">
         <v>1270</v>
       </c>
+      <c r="E20">
+        <f>1300000*B20</f>
+        <v>11700</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
@@ -1061,6 +1064,10 @@
       <c r="C22">
         <v>1270</v>
       </c>
+      <c r="E22">
+        <f>1300000/4</f>
+        <v>325000</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
@@ -1071,6 +1078,10 @@
       </c>
       <c r="C23" s="29">
         <v>0.1</v>
+      </c>
+      <c r="E23">
+        <f>1300000*4-(65000*4)</f>
+        <v>4940000</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
fixing single quote frontend page
</commit_message>
<xml_diff>
--- a/calc/static/piql_prices.xlsx
+++ b/calc/static/piql_prices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlfredoTrujillo\PycharmProjects\calculator\calc\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F3E634-7179-4018-B28C-32647667EEEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9D842D-008A-4972-B5A7-FB0DEB3D2E50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28935" yWindow="1605" windowWidth="14400" windowHeight="10320" tabRatio="781" xr2:uid="{D64C4359-5929-4BBC-9F5D-572B5F120BAE}"/>
   </bookViews>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD7F3CE-3398-4BFC-A88A-63EE7D330900}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.5"/>
@@ -1064,10 +1064,6 @@
       <c r="C22">
         <v>1270</v>
       </c>
-      <c r="E22">
-        <f>1300000/4</f>
-        <v>325000</v>
-      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
@@ -1078,10 +1074,6 @@
       </c>
       <c r="C23" s="29">
         <v>0.1</v>
-      </c>
-      <c r="E23">
-        <f>1300000*4-(65000*4)</f>
-        <v>4940000</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">

</xml_diff>